<commit_message>
Reduce Food for Hills, Marsh and Rainforests
</commit_message>
<xml_diff>
--- a/文档/地形地貌.xlsx
+++ b/文档/地形地貌.xlsx
@@ -1428,10 +1428,10 @@
   <sheetPr/>
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="H17" sqref="H17:K18"/>
+      <selection pane="topRight" activeCell="G12" sqref="G12:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9" s="4">
         <v>0</v>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="4">
         <v>0</v>
@@ -1740,7 +1740,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
Drop Gold reform experiment
AIs are way better at earning gold, and we should try to make commercial hub more important. Also let lakes produce more food
</commit_message>
<xml_diff>
--- a/文档/地形地貌.xlsx
+++ b/文档/地形地貌.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6250D04-3F10-480B-A4AE-35BAAF9E0104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A389F555-78E8-47A7-82DE-301B028576B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="4710" windowWidth="29475" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="119">
   <si>
     <t>地形类型</t>
   </si>
@@ -208,9 +208,6 @@
     <t>1粮，湖泊+2粮</t>
   </si>
   <si>
-    <t>通过科技加了1金</t>
-  </si>
-  <si>
     <t>TERRAIN_OCEAN</t>
   </si>
   <si>
@@ -238,251 +235,161 @@
     <t>FEATURE_FLOODPLAINS</t>
   </si>
   <si>
+    <t>（地形）3粮，+10%防御战斗力</t>
+  </si>
+  <si>
+    <t>+3粮</t>
+  </si>
+  <si>
+    <t>2粮，-10%防御战斗力</t>
+  </si>
+  <si>
+    <t>FEATURE_FLOODPLAINS_GRASSLAND</t>
+  </si>
+  <si>
+    <t>FEATURE_FLOODPLAINS_PLAINS</t>
+  </si>
+  <si>
+    <t>+1粮+1锤，洪水增产</t>
+  </si>
+  <si>
+    <t>FEATURE_JUNGLE</t>
+  </si>
+  <si>
+    <t>+1粮</t>
+  </si>
+  <si>
+    <t>（地形）1粮，2移动力，宝石4金，+50%防御战斗力</t>
+  </si>
+  <si>
+    <t>（地形）1粮，2移动力，+50%防御战斗力</t>
+  </si>
+  <si>
+    <t>（地形）1粮，3移动力，+25%防御战斗力</t>
+  </si>
+  <si>
+    <t>-1粮，2移动力，+50%防御战斗力，未改良时不能从河流获得金钱</t>
+  </si>
+  <si>
+    <t>（替代产出）2粮，2移动力，+25%防御战斗力</t>
+  </si>
+  <si>
+    <t>FEATURE_FOREST</t>
+  </si>
+  <si>
+    <t>+1锤</t>
+  </si>
+  <si>
+    <t>（地形）1粮2锤，2移动力，猎场资源+2粮，+50%防御战斗力</t>
+  </si>
+  <si>
+    <t>（地形）1粮2锤，2移动力，+50%防御战斗力</t>
+  </si>
+  <si>
+    <t>（地形）1粮2锤，2移动力，+25%防御战斗力</t>
+  </si>
+  <si>
+    <t>+1锤，2移动力，+50%防御战斗力，未改良时不能从河流获得金钱</t>
+  </si>
+  <si>
+    <t>（替代产出）1粮1锤，2移动力，+25%防御战斗力</t>
+  </si>
+  <si>
+    <t>历代文明中，除了文明5没有给它加产以外，基本上不约而同地给森林加了锤。我们就不调整了。</t>
+  </si>
+  <si>
+    <t>FEATURE_OASIS</t>
+  </si>
+  <si>
+    <t>+3粮+1金</t>
+  </si>
+  <si>
+    <t>+3粮+2金</t>
+  </si>
+  <si>
+    <t>（替代产出）3粮，-10%防御战斗力</t>
+  </si>
+  <si>
+    <t>FEATURE_MARSH</t>
+  </si>
+  <si>
+    <t>（地形）1粮，2移动力，石油4锤，+50%防御战斗力</t>
+  </si>
+  <si>
+    <t>（地形）1粮，2移动力，+20%防御战斗力</t>
+  </si>
+  <si>
+    <t>（替代产出）1粮，2移动力，-15%防御战斗力</t>
+  </si>
+  <si>
+    <t>加什么粮啊，减粮。沼泽只出现在草原上，所以无锤可减。</t>
+  </si>
+  <si>
+    <t>FEATURE_VOLCANO</t>
+  </si>
+  <si>
+    <t>（地形）3锤，3移动力，+80%防御战斗力</t>
+  </si>
+  <si>
+    <t>不变</t>
+  </si>
+  <si>
+    <t>FEATURE_REEF</t>
+  </si>
+  <si>
+    <t>+1粮+1锤</t>
+  </si>
+  <si>
+    <t>（替代产出）2粮1锤</t>
+  </si>
+  <si>
+    <t>FEATURE_ICE</t>
+  </si>
+  <si>
+    <t>FEATURE_GEOTHERMAL_FISSURE</t>
+  </si>
+  <si>
+    <t>FEATURE_VOLCANIC_SOIL</t>
+  </si>
+  <si>
+    <t>FEATURE_BURNING_FOREST</t>
+  </si>
+  <si>
+    <t>FEATURE_BURNT_FOREST</t>
+  </si>
+  <si>
+    <t>FEATURE_BURNING_JUNGLE</t>
+  </si>
+  <si>
+    <t>FEATURE_BURNT_JUNGLE</t>
+  </si>
+  <si>
+    <t>历代文明要么减粮，要么减锤，至少也没有额外产出，还有修建改良设施的额外惩罚时间。考虑到无粮的丘陵上减粮比较奇怪，我们就设置它为0产吧。毕竟雨林带真的不那么适合人类生存。也符合绝大多数雨林国家毁林才能开发的历史事实。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文明5的做法是使用了贸易路线功能替代了河流和海岸的金。我们可以看一下金是否是加得有点多了。
+用科技给湖泊+1粮吧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>+2粮，洪水增产</t>
-  </si>
-  <si>
-    <t>（地形）3粮，+10%防御战斗力</t>
-  </si>
-  <si>
-    <t>+3粮</t>
-  </si>
-  <si>
-    <t>2粮，-10%防御战斗力</t>
-  </si>
-  <si>
-    <t>FEATURE_FLOODPLAINS_GRASSLAND</t>
-  </si>
-  <si>
-    <t>FEATURE_FLOODPLAINS_PLAINS</t>
-  </si>
-  <si>
-    <t>+1粮+1锤，洪水增产</t>
-  </si>
-  <si>
-    <t>FEATURE_JUNGLE</t>
-  </si>
-  <si>
-    <t>+1粮</t>
-  </si>
-  <si>
-    <t>（地形）1粮，2移动力，宝石4金，+50%防御战斗力</t>
-  </si>
-  <si>
-    <t>（地形）1粮，2移动力，+50%防御战斗力</t>
-  </si>
-  <si>
-    <t>（地形）1粮，3移动力，+25%防御战斗力</t>
-  </si>
-  <si>
-    <t>-1粮，2移动力，+50%防御战斗力，未改良时不能从河流获得金钱</t>
-  </si>
-  <si>
-    <t>（替代产出）2粮，2移动力，+25%防御战斗力</t>
-  </si>
-  <si>
-    <t>历代文明要么减粮，要么减锤，至少也没有额外产出，还有修建改良设施的额外惩罚时间。我们参照文明4对它进行一个粮的减（如果在无粮的丘陵上减粮不会创死游戏的话）。毕竟雨林带真的不那么适合人类生存。也符合绝大多数雨林国家毁林才能开发的历史事实。</t>
-  </si>
-  <si>
-    <t>FEATURE_FOREST</t>
-  </si>
-  <si>
-    <t>+1锤</t>
-  </si>
-  <si>
-    <t>（地形）1粮2锤，2移动力，猎场资源+2粮，+50%防御战斗力</t>
-  </si>
-  <si>
-    <t>（地形）1粮2锤，2移动力，+50%防御战斗力</t>
-  </si>
-  <si>
-    <t>（地形）1粮2锤，2移动力，+25%防御战斗力</t>
-  </si>
-  <si>
-    <t>+1锤，2移动力，+50%防御战斗力，未改良时不能从河流获得金钱</t>
-  </si>
-  <si>
-    <t>（替代产出）1粮1锤，2移动力，+25%防御战斗力</t>
-  </si>
-  <si>
-    <t>历代文明中，除了文明5没有给它加产以外，基本上不约而同地给森林加了锤。我们就不调整了。</t>
-  </si>
-  <si>
-    <t>FEATURE_OASIS</t>
-  </si>
-  <si>
-    <t>+3粮+1金</t>
-  </si>
-  <si>
-    <t>+3粮+2金</t>
-  </si>
-  <si>
-    <t>（替代产出）3粮，-10%防御战斗力</t>
-  </si>
-  <si>
-    <t>FEATURE_MARSH</t>
-  </si>
-  <si>
-    <t>（地形）1粮，2移动力，石油4锤，+50%防御战斗力</t>
-  </si>
-  <si>
-    <t>（地形）1粮，2移动力，+20%防御战斗力</t>
-  </si>
-  <si>
-    <t>（替代产出）1粮，2移动力，-15%防御战斗力</t>
-  </si>
-  <si>
-    <t>加什么粮啊，减粮。沼泽只出现在草原上，所以无锤可减。</t>
-  </si>
-  <si>
-    <t>FEATURE_VOLCANO</t>
-  </si>
-  <si>
-    <t>（地形）3锤，3移动力，+80%防御战斗力</t>
-  </si>
-  <si>
-    <t>不变</t>
-  </si>
-  <si>
-    <t>FEATURE_REEF</t>
-  </si>
-  <si>
-    <t>+1粮+1锤</t>
-  </si>
-  <si>
-    <t>（替代产出）2粮1锤</t>
-  </si>
-  <si>
-    <t>FEATURE_ICE</t>
-  </si>
-  <si>
-    <t>FEATURE_GEOTHERMAL_FISSURE</t>
-  </si>
-  <si>
-    <t>FEATURE_VOLCANIC_SOIL</t>
-  </si>
-  <si>
-    <t>FEATURE_BURNING_FOREST</t>
-  </si>
-  <si>
-    <t>FEATURE_BURNT_FOREST</t>
-  </si>
-  <si>
-    <t>FEATURE_BURNING_JUNGLE</t>
-  </si>
-  <si>
-    <t>FEATURE_BURNT_JUNGLE</t>
-  </si>
-  <si>
-    <t>自然奇观</t>
-  </si>
-  <si>
-    <t>FEATURE_BARRIER_REEF</t>
-  </si>
-  <si>
-    <t>FEATURE_CLIFFS_DOVER</t>
-  </si>
-  <si>
-    <t>FEATURE_CRATER_LAKE</t>
-  </si>
-  <si>
-    <t>FEATURE_DEAD_SEA</t>
-  </si>
-  <si>
-    <t>FEATURE_EVEREST</t>
-  </si>
-  <si>
-    <t>FEATURE_GALAPAGOS</t>
-  </si>
-  <si>
-    <t>FEATURE_KILIMANJARO</t>
-  </si>
-  <si>
-    <t>FEATURE_PANTANAL</t>
-  </si>
-  <si>
-    <t>FEATURE_PIOPIOTAHI</t>
-  </si>
-  <si>
-    <t>FEATURE_TORRES_DEL_PAINE</t>
-  </si>
-  <si>
-    <t>FEATURE_TSINGY</t>
-  </si>
-  <si>
-    <t>FEATURE_YOSEMITE</t>
-  </si>
-  <si>
-    <t>FEATURE_HA_LONG_BAY</t>
-  </si>
-  <si>
-    <t>FEATURE_EYJAFJALLAJOKULL</t>
-  </si>
-  <si>
-    <t>FEATURE_LYSEFJORDEN</t>
-  </si>
-  <si>
-    <t>FEATURE_GIANTS_CAUSEWAY</t>
-  </si>
-  <si>
-    <t>FEATURE_ULURU</t>
-  </si>
-  <si>
-    <t>FEATURE_DELICATE_ARCH</t>
-  </si>
-  <si>
-    <t>FEATURE_EYE_OF_THE_SAHARA</t>
-  </si>
-  <si>
-    <t>FEATURE_LAKE_RETBA</t>
-  </si>
-  <si>
-    <t>FEATURE_MATTERHORN</t>
-  </si>
-  <si>
-    <t>FEATURE_RORAIMA</t>
-  </si>
-  <si>
-    <t>FEATURE_UBSUNUR_HOLLOW</t>
-  </si>
-  <si>
-    <t>FEATURE_ZHANGYE_DANXIA</t>
-  </si>
-  <si>
-    <t>FEATURE_CHOCOLATEHILLS</t>
-  </si>
-  <si>
-    <t>FEATURE_DEVILSTOWER</t>
-  </si>
-  <si>
-    <t>FEATURE_GOBUSTAN</t>
-  </si>
-  <si>
-    <t>FEATURE_IKKIL</t>
-  </si>
-  <si>
-    <t>FEATURE_PAMUKKALE</t>
-  </si>
-  <si>
-    <t>FEATURE_VESUVIUS</t>
-  </si>
-  <si>
-    <t>FEATURE_WHITEDESERT</t>
-  </si>
-  <si>
-    <t>FEATURE_BERMUDA_TRIANGLE</t>
-  </si>
-  <si>
-    <t>FEATURE_FOUNTAIN_OF_YOUTH</t>
-  </si>
-  <si>
-    <t>FEATURE_PAITITI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙漠泛滥平原提供了额外2粮和洪水增产的潜力，草原和平原也应该额外提供一些产出。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,6 +400,14 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -519,7 +434,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -543,6 +458,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -819,11 +746,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G12" sqref="G12:G16"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E20" sqref="E20:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -836,7 +763,8 @@
     <col min="6" max="6" width="19" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
     <col min="8" max="8" width="46.25" customWidth="1"/>
-    <col min="9" max="11" width="3.25" customWidth="1"/>
+    <col min="9" max="9" width="4.25" customWidth="1"/>
+    <col min="10" max="11" width="3.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
@@ -1249,16 +1177,22 @@
       <c r="G17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="H17" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>24</v>
@@ -1266,83 +1200,99 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="F20" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="G20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="H20" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20" s="3">
+        <v>2</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1353,55 +1303,67 @@
       <c r="G21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="3">
+        <v>2</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="3">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="F23" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>86</v>
+      <c r="H23" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="I23" s="3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="3">
         <v>0</v>
@@ -1412,28 +1374,28 @@
     </row>
     <row r="24" spans="1:11" ht="54" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="E24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="F24" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="H24" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -1441,25 +1403,25 @@
     </row>
     <row r="25" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>51</v>
@@ -1470,28 +1432,28 @@
     </row>
     <row r="26" spans="1:11" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="I26" s="3">
         <v>-1</v>
@@ -1505,7 +1467,7 @@
     </row>
     <row r="27" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>30</v>
@@ -1517,7 +1479,7 @@
         <v>30</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>30</v>
@@ -1526,7 +1488,7 @@
         <v>30</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
@@ -1534,10 +1496,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>30</v>
@@ -1552,10 +1514,10 @@
         <v>30</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
@@ -1563,7 +1525,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>46</v>
@@ -1584,7 +1546,7 @@
         <v>46</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
@@ -1592,7 +1554,7 @@
     </row>
     <row r="30" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="2"/>
@@ -1607,7 +1569,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="2"/>
@@ -1622,7 +1584,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="2"/>
@@ -1637,7 +1599,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="2"/>
@@ -1652,7 +1614,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="2"/>
@@ -1667,7 +1629,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="2"/>
@@ -1680,541 +1642,14 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A36" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A37" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A38" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A39" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A40" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A41" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A42" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A43" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A44" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A45" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A46" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A47" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A48" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A49" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A50" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A51" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A52" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A53" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A54" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-    </row>
-    <row r="55" spans="1:11" ht="27" x14ac:dyDescent="0.15">
-      <c r="A55" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A56" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A57" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A58" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A59" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A60" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A61" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A62" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A63" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A64" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A65" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A66" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A67" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A68" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-    </row>
-    <row r="69" spans="1:11" ht="27" x14ac:dyDescent="0.15">
-      <c r="A69" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A70" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-      <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="H2:K6"/>
-    <mergeCell ref="H20:K22"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G12:G16"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="H12:K16"/>
-    <mergeCell ref="H17:K18"/>
+  <mergeCells count="28">
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H20:H22"/>
     <mergeCell ref="H29:K29"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C7:C11"/>
@@ -2231,11 +1666,12 @@
     <mergeCell ref="F7:F11"/>
     <mergeCell ref="F12:F16"/>
     <mergeCell ref="F21:F22"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H2:K6"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G12:G16"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="H12:K16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>